<commit_message>
fixed messaging and grammer issues in form
</commit_message>
<xml_diff>
--- a/educational_modules/forms/app/covid_education.xlsx
+++ b/educational_modules/forms/app/covid_education.xlsx
@@ -328,7 +328,7 @@
     <t>sneezing_coughing_q</t>
   </si>
   <si>
-    <t>What is the best way to cover your cough?</t>
+    <t xml:space="preserve">What is the best way to cover your cough? </t>
   </si>
   <si>
     <t>select_one household</t>
@@ -382,7 +382,7 @@
     <t>hand_washing_sug</t>
   </si>
   <si>
-    <t>&lt;span style=“color:red”&gt;- Handwashing (and it’s ability to prevent COVID)&lt;/span&gt;</t>
+    <t>&lt;span style=“color:red”&gt;- Handwashing (and its ability to prevent COVID)&lt;/span&gt;</t>
   </si>
   <si>
     <t>${hand_washing_q} != ‘both_soap_and_water_or_hand_saniter’</t>
@@ -418,7 +418,7 @@
     <t>social_distancing_sug</t>
   </si>
   <si>
-    <t>&lt;span style=“color:red”&gt;- Social Distancing&lt;/span&gt;</t>
+    <t>&lt;span style=“color:red”&gt;- Social Distancing &lt;/span&gt;</t>
   </si>
   <si>
     <t>${social_distancing_q} != ‘at_least_2_meters’</t>
@@ -433,7 +433,7 @@
     <t>hand_washing_pass</t>
   </si>
   <si>
-    <t>&lt;span style=“color:green”&gt;- Handwashing (and it’s ability to prevent COVID)&lt;/span&gt;</t>
+    <t>&lt;span style=“color:green”&gt;- Handwashing (and its ability to prevent COVID)&lt;/span&gt;</t>
   </si>
   <si>
     <t>${hand_washing_q} = ‘both_soap_and_water_or_hand_saniter’</t>
@@ -451,7 +451,7 @@
     <t>sneezing_coughing_pass</t>
   </si>
   <si>
-    <t>&lt;span style=“color:green”&gt;- Sneezing/Coughing&lt;/span&gt;</t>
+    <t>&lt;span style=“color:green”&gt;- Sneezing/Coughing &lt;/span&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">${sneezing_coughing_q} = ‘cough_into_your_elbow_or_tissue’ </t>
@@ -7790,7 +7790,7 @@
       </c>
       <c r="C2" s="70">
         <f>NOW()</f>
-        <v>43961.865972222222</v>
+        <v>43968.949537037035</v>
       </c>
       <c r="D2" t="s" s="65">
         <v>194</v>

</xml_diff>